<commit_message>
Update excel sheet of investments and expenses
</commit_message>
<xml_diff>
--- a/Component List Robot Design.xlsx
+++ b/Component List Robot Design.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\GitRepos\Autonomous-Mobile-Robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>LM2596S 3-40V to 1.5-35V 4A DC to DC Adjustable Step-Down Buck Module</t>
   </si>
@@ -120,6 +120,21 @@
   </si>
   <si>
     <t>CB3D</t>
+  </si>
+  <si>
+    <t>Power Supply base Laser cut,</t>
+  </si>
+  <si>
+    <t>Lasercutting.lk</t>
+  </si>
+  <si>
+    <t>spacers</t>
+  </si>
+  <si>
+    <t>Scion</t>
+  </si>
+  <si>
+    <t>Gripper Base, Arm base 3D Print</t>
   </si>
 </sst>
 </file>
@@ -187,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,12 +234,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -360,7 +369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -377,10 +386,9 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="6" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -674,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,61 +696,55 @@
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.6640625" customWidth="1"/>
-    <col min="10" max="10" width="19.88671875" customWidth="1"/>
+    <col min="10" max="10" width="27.88671875" customWidth="1"/>
     <col min="11" max="11" width="20.21875" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="17"/>
+      <c r="F1" s="16"/>
       <c r="I1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="19" t="s">
         <v>14</v>
       </c>
       <c r="K1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-    </row>
-    <row r="2" spans="1:13" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+    </row>
+    <row r="2" spans="1:11" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
       <c r="I2" s="7"/>
       <c r="J2" s="9"/>
       <c r="K2" s="11"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-    </row>
-    <row r="3" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
+    </row>
+    <row r="3" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="21"/>
+      <c r="F3" s="20"/>
       <c r="I3" s="5" t="s">
         <v>11</v>
       </c>
@@ -752,16 +754,14 @@
       <c r="K3" s="10">
         <v>5000</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-    </row>
-    <row r="4" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
+    </row>
+    <row r="4" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="21"/>
+      <c r="F4" s="20"/>
       <c r="I4" s="5" t="s">
         <v>16</v>
       </c>
@@ -771,14 +771,12 @@
       <c r="K4" s="10">
         <v>3000</v>
       </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-    </row>
-    <row r="5" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
+    </row>
+    <row r="5" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="21">
         <v>150</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -791,7 +789,7 @@
         <f>B5*D5</f>
         <v>600</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="20"/>
       <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
@@ -801,14 +799,12 @@
       <c r="K5" s="10">
         <v>1000</v>
       </c>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-    </row>
-    <row r="6" spans="1:13" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="6" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="21">
         <v>1950</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -818,10 +814,10 @@
         <v>1</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" ref="E6:E16" si="0">B6*D6</f>
+        <f t="shared" ref="E6:E18" si="0">B6*D6</f>
         <v>1950</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="20"/>
       <c r="I6" s="7" t="s">
         <v>18</v>
       </c>
@@ -831,11 +827,9 @@
       <c r="K6" s="11">
         <v>2000</v>
       </c>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-    </row>
-    <row r="7" spans="1:13" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="23" t="s">
+    </row>
+    <row r="7" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="22" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="3">
@@ -851,13 +845,13 @@
         <f t="shared" si="0"/>
         <v>2950</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="20"/>
       <c r="I7" s="5"/>
       <c r="J7" s="6"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A8" s="23" t="s">
+    <row r="8" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A8" s="22" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="3">
@@ -873,18 +867,18 @@
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="20"/>
       <c r="I8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="17">
         <v>44102</v>
       </c>
       <c r="K8" s="15">
         <v>3000</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -901,7 +895,7 @@
         <f>B9*D9</f>
         <v>560</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="20"/>
       <c r="I9" s="5" t="s">
         <v>20</v>
       </c>
@@ -912,7 +906,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -929,12 +923,12 @@
         <f>B10*D10</f>
         <v>1900</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="20"/>
       <c r="I10" s="7"/>
       <c r="J10" s="8"/>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -951,12 +945,12 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="F11" s="21"/>
+      <c r="F11" s="20"/>
       <c r="I11" s="7"/>
       <c r="J11" s="8"/>
       <c r="K11" s="11"/>
     </row>
-    <row r="12" spans="1:13" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -973,18 +967,18 @@
         <f t="shared" si="0"/>
         <v>1850</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="I12" s="24" t="s">
+      <c r="F12" s="20"/>
+      <c r="I12" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="24">
         <v>44104</v>
       </c>
-      <c r="K12" s="26">
+      <c r="K12" s="25">
         <v>800</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -1001,12 +995,12 @@
         <f t="shared" si="0"/>
         <v>7700</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="26"/>
-    </row>
-    <row r="14" spans="1:13" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F13" s="20"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="25"/>
+    </row>
+    <row r="14" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
@@ -1023,18 +1017,18 @@
         <f t="shared" si="0"/>
         <v>715</v>
       </c>
-      <c r="F14" s="21"/>
+      <c r="F14" s="20"/>
       <c r="I14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="17">
         <v>44110</v>
       </c>
       <c r="K14" s="15">
         <v>1015</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -1051,12 +1045,12 @@
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="26"/>
-    </row>
-    <row r="16" spans="1:13" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F15" s="20"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="25"/>
+    </row>
+    <row r="16" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1073,7 +1067,7 @@
         <f t="shared" si="0"/>
         <v>320</v>
       </c>
-      <c r="F16" s="21"/>
+      <c r="F16" s="20"/>
       <c r="I16" s="7" t="s">
         <v>18</v>
       </c>
@@ -1084,61 +1078,155 @@
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="21"/>
-    </row>
-    <row r="18" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="21"/>
+    <row r="17" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="3">
+        <v>300</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="F17" s="20"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="25"/>
+    </row>
+    <row r="18" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="3">
+        <v>265</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>265</v>
+      </c>
+      <c r="F18" s="20"/>
+      <c r="I18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="8">
+        <v>44112</v>
+      </c>
+      <c r="K18" s="11">
+        <v>565</v>
+      </c>
     </row>
     <row r="19" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="21"/>
-    </row>
-    <row r="20" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="21"/>
+      <c r="A19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3">
+        <v>3390</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <f>B19*D19</f>
+        <v>3390</v>
+      </c>
+      <c r="F19" s="20"/>
+    </row>
+    <row r="20" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="20"/>
     </row>
     <row r="21" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A28" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13">
-        <f>SUM(E5:E16)</f>
-        <v>20565</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="I22" s="19" t="s">
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13">
+        <f>SUM(E5:E27)</f>
+        <v>24520</v>
+      </c>
+      <c r="I28" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19">
-        <f>SUM(K3:K19)</f>
-        <v>21135</v>
-      </c>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18">
+        <f>SUM(K3:K27)</f>
+        <v>21700</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Laser cut arm base, update inv and exp excel sheet
</commit_message>
<xml_diff>
--- a/Component List Robot Design.xlsx
+++ b/Component List Robot Design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>LM2596S 3-40V to 1.5-35V 4A DC to DC Adjustable Step-Down Buck Module</t>
   </si>
@@ -134,14 +134,23 @@
     <t>Scion</t>
   </si>
   <si>
-    <t>Gripper Base, Arm base 3D Print</t>
+    <t>Gripper Base 3D Print</t>
+  </si>
+  <si>
+    <t>Arm base laser cut</t>
+  </si>
+  <si>
+    <t>3mm Nuts and bolts</t>
+  </si>
+  <si>
+    <t>Anakade(pvt) Ltd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +210,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Adobe Heiti Std R"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -222,12 +238,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -238,8 +248,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -360,6 +376,74 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -369,27 +453,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="6" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -397,10 +470,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="9" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="9" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="9" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -685,14 +773,14 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="111.88671875" customWidth="1"/>
     <col min="2" max="2" width="22.21875" customWidth="1"/>
-    <col min="3" max="3" width="25.21875" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.6640625" customWidth="1"/>
@@ -701,82 +789,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="I1" s="14" t="s">
+      <c r="F1" s="7"/>
+      <c r="I1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="17"/>
+    </row>
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="20"/>
-      <c r="I3" s="5" t="s">
+      <c r="F3" s="9"/>
+      <c r="I3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="19">
         <v>44098</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="20">
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="20"/>
-      <c r="I4" s="5" t="s">
+      <c r="F4" s="9"/>
+      <c r="I4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="19">
         <v>44099</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="20">
         <v>3000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="10">
         <v>150</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -789,22 +877,22 @@
         <f>B5*D5</f>
         <v>600</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="I5" s="5" t="s">
+      <c r="F5" s="9"/>
+      <c r="I5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="19">
         <v>44099</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="20">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="10">
         <v>1950</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -817,19 +905,19 @@
         <f t="shared" ref="E6:E18" si="0">B6*D6</f>
         <v>1950</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="I6" s="7" t="s">
+      <c r="F6" s="9"/>
+      <c r="I6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="21">
         <v>44099</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="17">
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="22" t="s">
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="3">
@@ -845,13 +933,19 @@
         <f t="shared" si="0"/>
         <v>2950</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="10"/>
-    </row>
-    <row r="8" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A8" s="22" t="s">
+      <c r="F7" s="9"/>
+      <c r="I7" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="29">
+        <v>44102</v>
+      </c>
+      <c r="K7" s="28">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A8" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="3">
@@ -867,18 +961,18 @@
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="I8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="17">
+      <c r="F8" s="9"/>
+      <c r="I8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="19">
         <v>44102</v>
       </c>
-      <c r="K8" s="15">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="K8" s="20">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -895,18 +989,18 @@
         <f>B9*D9</f>
         <v>560</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="I9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="6">
-        <v>44102</v>
-      </c>
-      <c r="K9" s="10">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F9" s="9"/>
+      <c r="I9" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="23">
+        <v>44104</v>
+      </c>
+      <c r="K9" s="24">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -923,12 +1017,18 @@
         <f>B10*D10</f>
         <v>1900</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="11"/>
-    </row>
-    <row r="11" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F10" s="9"/>
+      <c r="I10" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="29">
+        <v>44110</v>
+      </c>
+      <c r="K10" s="28">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -945,12 +1045,18 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="11"/>
-    </row>
-    <row r="12" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F11" s="9"/>
+      <c r="I11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="21">
+        <v>44111</v>
+      </c>
+      <c r="K11" s="17">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -967,18 +1073,18 @@
         <f t="shared" si="0"/>
         <v>1850</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="I12" s="23" t="s">
+      <c r="F12" s="9"/>
+      <c r="I12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="24">
-        <v>44104</v>
-      </c>
-      <c r="K12" s="25">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J12" s="21">
+        <v>44112</v>
+      </c>
+      <c r="K12" s="17">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -995,12 +1101,18 @@
         <f t="shared" si="0"/>
         <v>7700</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="25"/>
-    </row>
-    <row r="14" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F13" s="9"/>
+      <c r="I13" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="29">
+        <v>44118</v>
+      </c>
+      <c r="K13" s="28">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
@@ -1017,18 +1129,16 @@
         <f t="shared" si="0"/>
         <v>715</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="I14" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="17">
-        <v>44110</v>
-      </c>
-      <c r="K14" s="15">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F14" s="9"/>
+      <c r="I14" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="30"/>
+      <c r="K14" s="26">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -1045,12 +1155,9 @@
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="25"/>
-    </row>
-    <row r="16" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1067,18 +1174,9 @@
         <f t="shared" si="0"/>
         <v>320</v>
       </c>
-      <c r="F16" s="20"/>
-      <c r="I16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="8">
-        <v>44111</v>
-      </c>
-      <c r="K16" s="11">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -1095,12 +1193,9 @@
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="F17" s="20"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="25"/>
-    </row>
-    <row r="18" spans="1:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
@@ -1117,23 +1212,14 @@
         <f t="shared" si="0"/>
         <v>265</v>
       </c>
-      <c r="F18" s="20"/>
-      <c r="I18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="8">
-        <v>44112</v>
-      </c>
-      <c r="K18" s="11">
-        <v>565</v>
-      </c>
+      <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="3">
-        <v>3390</v>
+        <v>1100</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>31</v>
@@ -1143,31 +1229,61 @@
       </c>
       <c r="E19" s="3">
         <f>B19*D19</f>
-        <v>3390</v>
-      </c>
-      <c r="F19" s="20"/>
+        <v>1100</v>
+      </c>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="20"/>
+      <c r="A20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="3">
+        <v>500</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <f>B20*D20</f>
+        <v>500</v>
+      </c>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="3">
+        <v>420</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
+        <f>B21*D21</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
+      <c r="I22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8">
+        <f>SUM(K3:K21)</f>
+        <v>23720</v>
+      </c>
     </row>
     <row r="23" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A23" s="3"/>
@@ -1204,24 +1320,16 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A28" s="12" t="s">
+    <row r="28" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6">
         <f>SUM(E5:E27)</f>
-        <v>24520</v>
-      </c>
-      <c r="I28" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18">
-        <f>SUM(K3:K27)</f>
-        <v>21700</v>
+        <v>23150</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">

</xml_diff>